<commit_message>
Allow callers to request information (value, formula, etc.) on cells that might not exist in the document.
</commit_message>
<xml_diff>
--- a/test/files/style.xlsx
+++ b/test/files/style.xlsx
@@ -1,17 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="25306"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="30" windowWidth="19935" windowHeight="9915"/>
+    <workbookView xWindow="480" yWindow="40" windowWidth="19940" windowHeight="9920"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="125725" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -51,8 +56,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="7">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -132,7 +137,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -140,6 +145,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -433,19 +439,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -457,6 +463,9 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
+      <c r="B2" s="7">
+        <v>1.26</v>
+      </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
@@ -506,30 +515,45 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>